<commit_message>
updated for Spanish GP
</commit_message>
<xml_diff>
--- a/fantasygp.xlsx
+++ b/fantasygp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b62176f68eb117a/Documents/developer/github.com/squirke1/fantasygp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="635" documentId="8_{A68CD679-44BD-9E44-A494-0D19E446F524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{701E1E77-FC1A-DD4A-87D5-0F0181F2535E}"/>
+  <xr:revisionPtr revIDLastSave="649" documentId="8_{A68CD679-44BD-9E44-A494-0D19E446F524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{670E2396-A735-4941-B762-4AD76F00E176}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{16E4FC74-DCF6-BE49-A5A5-1134F32D647F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="2" xr2:uid="{16E4FC74-DCF6-BE49-A5A5-1134F32D647F}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring" sheetId="5" r:id="rId1"/>
@@ -1536,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE4FC977-EE0F-F648-BFCF-D8797BF030EA}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2203,7 +2203,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="E2">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>8.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="E3">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>13</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2283,7 +2283,7 @@
       </c>
       <c r="E4">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="E5">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="E6">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2337,7 +2337,7 @@
       </c>
       <c r="E7">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>21</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="E8">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>6</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="E9">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2391,7 +2391,7 @@
       </c>
       <c r="E10">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="E11">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="E12">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>19</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="E13">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E14">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>17.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="E15">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="E16">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2517,7 +2517,7 @@
       </c>
       <c r="E17">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>8.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="E18">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>19.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="E19">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>12</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="E20">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>28</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="E21">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="E22">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="E23">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2643,7 +2643,7 @@
       </c>
       <c r="E24">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="E25">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2679,7 +2679,7 @@
       </c>
       <c r="E26">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>7</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="E27">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>6.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2733,7 +2733,7 @@
       </c>
       <c r="E29">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>5.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2751,7 +2751,7 @@
       </c>
       <c r="E30">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="E31">
         <f>Table2811[[#This Row],[Price]]</f>
-        <v>5.5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2784,7 +2784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E892A3-9A29-BC41-85E1-6E3BF7063D8E}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -2830,27 +2830,27 @@
       </c>
       <c r="B2">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="D2">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="E2">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>438</v>
+        <v>484</v>
       </c>
       <c r="F2">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>38.75</v>
+        <v>44.980000000000004</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -2862,27 +2862,27 @@
       </c>
       <c r="B3">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="C3">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="D3">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E3">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>572</v>
+        <v>627</v>
       </c>
       <c r="F3">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>13</v>
+        <v>12.5</v>
       </c>
       <c r="G3">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>35.950000000000003</v>
+        <v>40.6</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
@@ -2894,11 +2894,11 @@
       </c>
       <c r="B4">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C4">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>262</v>
+        <v>308</v>
       </c>
       <c r="D4">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -2906,15 +2906,15 @@
       </c>
       <c r="E4">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>384</v>
+        <v>435</v>
       </c>
       <c r="F4">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="G4">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>33.33</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="H4" t="s">
         <v>48</v>
@@ -2926,11 +2926,11 @@
       </c>
       <c r="B5">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>320</v>
+        <v>338</v>
       </c>
       <c r="C5">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>252</v>
+        <v>290</v>
       </c>
       <c r="D5">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -2938,15 +2938,15 @@
       </c>
       <c r="E5">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>572</v>
+        <v>628</v>
       </c>
       <c r="F5">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="G5">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>40.28</v>
+        <v>45.680000000000007</v>
       </c>
       <c r="H5" t="s">
         <v>48</v>
@@ -2962,23 +2962,23 @@
       </c>
       <c r="C6">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="D6">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E6">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>317</v>
+        <v>377</v>
       </c>
       <c r="F6">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G6">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>43.8</v>
+        <v>49.43</v>
       </c>
       <c r="H6" t="s">
         <v>0</v>
@@ -2990,11 +2990,11 @@
       </c>
       <c r="B7">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>557</v>
+        <v>658</v>
       </c>
       <c r="C7">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="D7">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3002,15 +3002,15 @@
       </c>
       <c r="E7">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>764</v>
+        <v>885</v>
       </c>
       <c r="F7">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>21</v>
+        <v>21.5</v>
       </c>
       <c r="G7">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>37.07</v>
+        <v>42.480000000000004</v>
       </c>
       <c r="H7" t="s">
         <v>48</v>
@@ -3022,27 +3022,27 @@
       </c>
       <c r="B8">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="D8">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="E8">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>357</v>
+        <v>416</v>
       </c>
       <c r="F8">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="G8">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>36.1</v>
+        <v>42.97</v>
       </c>
       <c r="H8" t="s">
         <v>0</v>
@@ -3054,11 +3054,11 @@
       </c>
       <c r="B9">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>239</v>
+        <v>276</v>
       </c>
       <c r="D9">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3066,15 +3066,15 @@
       </c>
       <c r="E9">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>257</v>
+        <v>295</v>
       </c>
       <c r="F9">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="G9">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>41.29</v>
+        <v>47.85</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
@@ -3086,11 +3086,11 @@
       </c>
       <c r="B10">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>253</v>
+        <v>289</v>
       </c>
       <c r="C10">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="D10">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3098,15 +3098,15 @@
       </c>
       <c r="E10">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>564</v>
+        <v>624</v>
       </c>
       <c r="F10">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>29.81</v>
+        <v>33.950000000000003</v>
       </c>
       <c r="H10" t="s">
         <v>0</v>
@@ -3118,27 +3118,27 @@
       </c>
       <c r="B11">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="D11">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="E11">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>291</v>
+        <v>351</v>
       </c>
       <c r="F11">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="G11">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>38.230000000000004</v>
+        <v>44.81</v>
       </c>
       <c r="H11" t="s">
         <v>0</v>
@@ -3150,27 +3150,27 @@
       </c>
       <c r="B12">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>282</v>
+        <v>344</v>
       </c>
       <c r="C12">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="D12">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="E12">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>571</v>
+        <v>688</v>
       </c>
       <c r="F12">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="G12">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>29.439999999999998</v>
+        <v>35.26</v>
       </c>
       <c r="H12" t="s">
         <v>0</v>
@@ -3186,23 +3186,23 @@
       </c>
       <c r="C13">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="D13">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E13">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>252</v>
+        <v>273</v>
       </c>
       <c r="F13">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="G13">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>39.119999999999997</v>
+        <v>44.449999999999996</v>
       </c>
       <c r="H13" t="s">
         <v>0</v>
@@ -3214,11 +3214,11 @@
       </c>
       <c r="B14">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>398</v>
+        <v>514</v>
       </c>
       <c r="C14">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="D14">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3226,15 +3226,15 @@
       </c>
       <c r="E14">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>637</v>
+        <v>781</v>
       </c>
       <c r="F14">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>17.5</v>
+        <v>20.5</v>
       </c>
       <c r="G14">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>38.14</v>
+        <v>44.06</v>
       </c>
       <c r="H14" t="s">
         <v>48</v>
@@ -3246,11 +3246,11 @@
       </c>
       <c r="B15">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>461</v>
+        <v>533</v>
       </c>
       <c r="C15">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>275</v>
+        <v>307</v>
       </c>
       <c r="D15">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3258,15 +3258,15 @@
       </c>
       <c r="E15">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>736</v>
+        <v>840</v>
       </c>
       <c r="F15">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
       <c r="G15">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>37.49</v>
+        <v>42.81</v>
       </c>
       <c r="H15" t="s">
         <v>48</v>
@@ -3278,27 +3278,27 @@
       </c>
       <c r="B16">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>263</v>
+        <v>336</v>
       </c>
       <c r="C16">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="D16">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="E16">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>588</v>
+        <v>701</v>
       </c>
       <c r="F16">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="G16">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>32.510000000000005</v>
+        <v>37.870000000000005</v>
       </c>
       <c r="H16" t="s">
         <v>0</v>
@@ -3310,27 +3310,27 @@
       </c>
       <c r="B17">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C17">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="D17">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E17">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>338</v>
+        <v>382</v>
       </c>
       <c r="F17">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="G17">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>33.81</v>
+        <v>39.85</v>
       </c>
       <c r="H17" t="s">
         <v>0</v>
@@ -3342,11 +3342,11 @@
       </c>
       <c r="B18">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>370</v>
+        <v>392</v>
       </c>
       <c r="C18">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D18">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3354,15 +3354,15 @@
       </c>
       <c r="E18">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>658</v>
+        <v>686</v>
       </c>
       <c r="F18">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>19.5</v>
+        <v>16</v>
       </c>
       <c r="G18">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>33.74</v>
+        <v>36.68</v>
       </c>
       <c r="H18" t="s">
         <v>0</v>
@@ -3374,27 +3374,27 @@
       </c>
       <c r="B19">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>135</v>
+        <v>178</v>
       </c>
       <c r="C19">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="D19">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E19">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>312</v>
+        <v>377</v>
       </c>
       <c r="F19">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="G19">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>24.3</v>
+        <v>29.32</v>
       </c>
       <c r="H19" t="s">
         <v>0</v>
@@ -3406,11 +3406,11 @@
       </c>
       <c r="B20">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>1055</v>
+        <v>1161</v>
       </c>
       <c r="C20">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>316</v>
+        <v>339</v>
       </c>
       <c r="D20">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3418,15 +3418,15 @@
       </c>
       <c r="E20">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>1371</v>
+        <v>1500</v>
       </c>
       <c r="F20">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>28</v>
+        <v>26.5</v>
       </c>
       <c r="G20">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>46.22</v>
+        <v>51.56</v>
       </c>
       <c r="H20" t="s">
         <v>48</v>
@@ -3438,27 +3438,27 @@
       </c>
       <c r="B21">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D21">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E21">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="F21">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="G21">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>38.590000000000003</v>
+        <v>44.06</v>
       </c>
       <c r="H21" t="s">
         <v>0</v>
@@ -3470,27 +3470,27 @@
       </c>
       <c r="B22">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>208</v>
+        <v>244</v>
       </c>
       <c r="C22">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="D22">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="E22">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>498</v>
+        <v>584</v>
       </c>
       <c r="F22">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="G22">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>31.340000000000003</v>
+        <v>36.21</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="B23">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="C23">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
@@ -3514,15 +3514,15 @@
       </c>
       <c r="E23">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>508</v>
+        <v>547</v>
       </c>
       <c r="F23">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G23">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>28.47</v>
+        <v>31.53</v>
       </c>
       <c r="H23" t="s">
         <v>0</v>
@@ -3538,23 +3538,23 @@
       </c>
       <c r="C24">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="D24">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E24">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="F24">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="G24">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>30.240000000000002</v>
+        <v>42.09</v>
       </c>
       <c r="H24" t="s">
         <v>0</v>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="C25">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>276</v>
+        <v>336</v>
       </c>
       <c r="D25">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3578,15 +3578,15 @@
       </c>
       <c r="E25">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>292</v>
+        <v>352</v>
       </c>
       <c r="F25">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G25">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>46.699999999999996</v>
+        <v>53.04</v>
       </c>
       <c r="H25" t="s">
         <v>48</v>
@@ -3598,27 +3598,27 @@
       </c>
       <c r="B26">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C26">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="D26">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E26">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>311</v>
+        <v>356</v>
       </c>
       <c r="F26">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="G26">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>32.99</v>
+        <v>38.57</v>
       </c>
       <c r="H26" t="s">
         <v>0</v>
@@ -3630,27 +3630,27 @@
       </c>
       <c r="B27">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C27">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>213</v>
+        <v>248</v>
       </c>
       <c r="D27">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E27">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>342</v>
+        <v>404</v>
       </c>
       <c r="F27">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="G27">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>42.089999999999996</v>
+        <v>50.4</v>
       </c>
       <c r="H27" t="s">
         <v>0</v>
@@ -3662,19 +3662,19 @@
       </c>
       <c r="B28">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>685</v>
+        <v>769</v>
       </c>
       <c r="C28">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="D28">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>330</v>
+        <v>375</v>
       </c>
       <c r="E28">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>1259</v>
+        <v>1415</v>
       </c>
       <c r="F28">
         <f>Table28[[#This Row],[Price]]</f>
@@ -3682,7 +3682,7 @@
       </c>
       <c r="G28">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>38.519999999999996</v>
+        <v>43.47</v>
       </c>
       <c r="H28" t="s">
         <v>0</v>
@@ -3694,11 +3694,11 @@
       </c>
       <c r="B29">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C29">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>245</v>
+        <v>285</v>
       </c>
       <c r="D29">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3706,15 +3706,15 @@
       </c>
       <c r="E29">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>277</v>
+        <v>338</v>
       </c>
       <c r="F29">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="G29">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>37.120000000000005</v>
+        <v>44.16</v>
       </c>
       <c r="H29" t="s">
         <v>48</v>
@@ -3726,11 +3726,11 @@
       </c>
       <c r="B30">
         <f>Table28[[#This Row],[Race]]+Table2[[#This Row],[Race]]</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>229</v>
+        <v>260</v>
       </c>
       <c r="D30">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
@@ -3738,15 +3738,15 @@
       </c>
       <c r="E30">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>257</v>
+        <v>290</v>
       </c>
       <c r="F30">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="G30">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>35.11</v>
+        <v>42.25</v>
       </c>
       <c r="H30" t="s">
         <v>48</v>
@@ -3762,23 +3762,23 @@
       </c>
       <c r="C31">
         <f>Table28[[#This Row],[Bonus]]+Table2[[#This Row],[Bonus]]</f>
-        <v>236</v>
+        <v>291</v>
       </c>
       <c r="D31">
         <f>Table28[[#This Row],[Qualy]]+Table2[[#This Row],[Qualy]]</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E31">
         <f>Table28[[#This Row],[Total]]+Table2[[#This Row],[Total]]</f>
-        <v>292</v>
+        <v>352</v>
       </c>
       <c r="F31">
         <f>Table28[[#This Row],[Price]]</f>
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="G31">
         <f>Table28[[#This Row],[Value]]+Table2[[#This Row],[Value]]</f>
-        <v>41.08</v>
+        <v>50.4</v>
       </c>
       <c r="H31" t="s">
         <v>0</v>
@@ -3797,7 +3797,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3841,22 +3841,22 @@
         <v>41</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E2">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="F2">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>7.65</v>
+        <v>13.88</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -3867,22 +3867,22 @@
         <v>27</v>
       </c>
       <c r="B3">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="F3">
-        <v>13</v>
+        <v>12.5</v>
       </c>
       <c r="G3">
-        <v>6.15</v>
+        <v>10.8</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
@@ -3893,22 +3893,22 @@
         <v>52</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="F4">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="G4">
-        <v>6.53</v>
+        <v>12.5</v>
       </c>
       <c r="H4" t="s">
         <v>48</v>
@@ -3919,22 +3919,22 @@
         <v>53</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C5">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="F5">
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="G5">
-        <v>6.08</v>
+        <v>11.48</v>
       </c>
       <c r="H5" t="s">
         <v>48</v>
@@ -3948,19 +3948,19 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>7.5</v>
+        <v>13.13</v>
       </c>
       <c r="H6" t="s">
         <v>0</v>
@@ -3971,22 +3971,22 @@
         <v>51</v>
       </c>
       <c r="B7">
-        <v>151</v>
+        <v>252</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>201</v>
+        <v>322</v>
       </c>
       <c r="F7">
-        <v>21</v>
+        <v>21.5</v>
       </c>
       <c r="G7">
-        <v>9.57</v>
+        <v>14.98</v>
       </c>
       <c r="H7" t="s">
         <v>48</v>
@@ -3997,22 +3997,22 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>11.87</v>
       </c>
       <c r="H8" t="s">
         <v>0</v>
@@ -4023,22 +4023,22 @@
         <v>57</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="G9">
-        <v>9.2899999999999991</v>
+        <v>15.85</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
@@ -4049,22 +4049,22 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="F10">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G10">
-        <v>3.11</v>
+        <v>7.25</v>
       </c>
       <c r="H10" t="s">
         <v>0</v>
@@ -4075,22 +4075,22 @@
         <v>43</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E11">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="F11">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="G11">
-        <v>8.1300000000000008</v>
+        <v>14.71</v>
       </c>
       <c r="H11" t="s">
         <v>0</v>
@@ -4101,22 +4101,22 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="C12">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="E12">
-        <v>128</v>
+        <v>245</v>
       </c>
       <c r="F12">
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="G12">
-        <v>6.74</v>
+        <v>12.56</v>
       </c>
       <c r="H12" t="s">
         <v>0</v>
@@ -4130,19 +4130,19 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D13">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="F13">
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="G13">
-        <v>6.82</v>
+        <v>12.15</v>
       </c>
       <c r="H13" t="s">
         <v>0</v>
@@ -4153,22 +4153,22 @@
         <v>58</v>
       </c>
       <c r="B14">
-        <v>96</v>
+        <v>212</v>
       </c>
       <c r="C14">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>132</v>
+        <v>276</v>
       </c>
       <c r="F14">
-        <v>17.5</v>
+        <v>20.5</v>
       </c>
       <c r="G14">
-        <v>7.54</v>
+        <v>13.46</v>
       </c>
       <c r="H14" t="s">
         <v>48</v>
@@ -4179,22 +4179,22 @@
         <v>50</v>
       </c>
       <c r="B15">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="C15">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="F15">
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
       <c r="G15">
-        <v>5.49</v>
+        <v>10.81</v>
       </c>
       <c r="H15" t="s">
         <v>48</v>
@@ -4205,22 +4205,22 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>58</v>
+        <v>131</v>
       </c>
       <c r="C16">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D16">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E16">
-        <v>114</v>
+        <v>227</v>
       </c>
       <c r="F16">
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="G16">
-        <v>6.91</v>
+        <v>12.27</v>
       </c>
       <c r="H16" t="s">
         <v>0</v>
@@ -4231,22 +4231,22 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E17">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="F17">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>8.7100000000000009</v>
+        <v>14.75</v>
       </c>
       <c r="H17" t="s">
         <v>0</v>
@@ -4257,22 +4257,22 @@
         <v>9</v>
       </c>
       <c r="B18">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="C18">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="F18">
-        <v>19.5</v>
+        <v>16</v>
       </c>
       <c r="G18">
-        <v>5.44</v>
+        <v>8.3800000000000008</v>
       </c>
       <c r="H18" t="s">
         <v>0</v>
@@ -4283,22 +4283,22 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C19">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E19">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="F19">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="G19">
-        <v>4.5</v>
+        <v>9.52</v>
       </c>
       <c r="H19" t="s">
         <v>0</v>
@@ -4309,22 +4309,22 @@
         <v>49</v>
       </c>
       <c r="B20">
-        <v>195</v>
+        <v>301</v>
       </c>
       <c r="C20">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>233</v>
+        <v>362</v>
       </c>
       <c r="F20">
-        <v>28</v>
+        <v>26.5</v>
       </c>
       <c r="G20">
-        <v>8.32</v>
+        <v>13.66</v>
       </c>
       <c r="H20" t="s">
         <v>48</v>
@@ -4335,22 +4335,22 @@
         <v>37</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E21">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="F21">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="G21">
-        <v>8.89</v>
+        <v>14.36</v>
       </c>
       <c r="H21" t="s">
         <v>0</v>
@@ -4361,22 +4361,22 @@
         <v>11</v>
       </c>
       <c r="B22">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C22">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D22">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E22">
-        <v>89</v>
+        <v>175</v>
       </c>
       <c r="F22">
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="G22">
-        <v>5.74</v>
+        <v>10.61</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -4387,7 +4387,7 @@
         <v>17</v>
       </c>
       <c r="B23">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="C23">
         <v>33</v>
@@ -4396,13 +4396,13 @@
         <v>15</v>
       </c>
       <c r="E23">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="F23">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G23">
-        <v>6.47</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="H23" t="s">
         <v>0</v>
@@ -4416,19 +4416,19 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="F24">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="G24">
-        <v>6.44</v>
+        <v>18.29</v>
       </c>
       <c r="H24" t="s">
         <v>0</v>
@@ -4442,19 +4442,19 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="F25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G25">
-        <v>7.8</v>
+        <v>14.14</v>
       </c>
       <c r="H25" t="s">
         <v>48</v>
@@ -4465,22 +4465,22 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E26">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="F26">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="G26">
-        <v>6.29</v>
+        <v>11.87</v>
       </c>
       <c r="H26" t="s">
         <v>0</v>
@@ -4491,22 +4491,22 @@
         <v>35</v>
       </c>
       <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>58</v>
+      </c>
+      <c r="D27">
+        <v>35</v>
+      </c>
+      <c r="E27">
+        <v>112</v>
+      </c>
+      <c r="F27">
         <v>7</v>
       </c>
-      <c r="C27">
-        <v>23</v>
-      </c>
-      <c r="D27">
-        <v>20</v>
-      </c>
-      <c r="E27">
-        <v>50</v>
-      </c>
-      <c r="F27">
-        <v>6.5</v>
-      </c>
       <c r="G27">
-        <v>7.69</v>
+        <v>16</v>
       </c>
       <c r="H27" t="s">
         <v>0</v>
@@ -4517,22 +4517,22 @@
         <v>7</v>
       </c>
       <c r="B28">
-        <v>110</v>
+        <v>194</v>
       </c>
       <c r="C28">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D28">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="E28">
-        <v>221</v>
+        <v>377</v>
       </c>
       <c r="F28">
         <v>31.5</v>
       </c>
       <c r="G28">
-        <v>7.02</v>
+        <v>11.97</v>
       </c>
       <c r="H28" t="s">
         <v>0</v>
@@ -4543,22 +4543,22 @@
         <v>85</v>
       </c>
       <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>76</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>104</v>
+      </c>
+      <c r="F29">
         <v>7</v>
       </c>
-      <c r="C29">
-        <v>36</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>43</v>
-      </c>
-      <c r="F29">
-        <v>5.5</v>
-      </c>
       <c r="G29">
-        <v>7.82</v>
+        <v>14.86</v>
       </c>
       <c r="H29" t="s">
         <v>48</v>
@@ -4569,22 +4569,22 @@
         <v>56</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="F30">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="G30">
-        <v>6.31</v>
+        <v>13.45</v>
       </c>
       <c r="H30" t="s">
         <v>48</v>
@@ -4598,19 +4598,19 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E31">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="F31">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="G31">
-        <v>8.18</v>
+        <v>17.5</v>
       </c>
       <c r="H31" t="s">
         <v>0</v>

</xml_diff>